<commit_message>
Updated Pride_Converter to support v2.x of the ProteomeXchange .px file format
</commit_message>
<xml_diff>
--- a/Plugins/AM_PRIDE_Converter_PlugIn/Docs/Submission_Px_Formatted.xlsx
+++ b/Plugins/AM_PRIDE_Converter_PlugIn/Docs/Submission_Px_Formatted.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="submission" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="73">
   <si>
     <t>MTD</t>
   </si>
@@ -206,6 +207,33 @@
   </si>
   <si>
     <t>technical replicate 2</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>affiliation</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>pride_login</t>
+  </si>
+  <si>
+    <t>-- removed --</t>
   </si>
 </sst>
 </file>
@@ -690,8 +718,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1036,9 +1068,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1468,4 +1498,144 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="str">
+        <f>"dctKeyNameOverrides.Add("""&amp;B1&amp;""""&amp;","&amp;""""&amp;C1&amp;""")"</f>
+        <v>dctKeyNameOverrides.Add("name","submitter_name")</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="str">
+        <f t="shared" ref="D2:D8" si="0">"dctKeyNameOverrides.Add("""&amp;B2&amp;""""&amp;","&amp;""""&amp;C2&amp;""")"</f>
+        <v>dctKeyNameOverrides.Add("email","submitter_email")</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>dctKeyNameOverrides.Add("affiliation","submitter_affiliation")</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>dctKeyNameOverrides.Add("title","project_title")</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>dctKeyNameOverrides.Add("description","project_description")</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>dctKeyNameOverrides.Add("type","submission_type")</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>dctKeyNameOverrides.Add("comment","-- removed --")</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>dctKeyNameOverrides.Add("pride_login","submitter_pride_login")</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>